<commit_message>
custom seed shop data
</commit_message>
<xml_diff>
--- a/db/seed/coopmartDN.xlsx
+++ b/db/seed/coopmartDN.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baoqu\OneDrive\Desktop\DATN\IndoorMapServer\db\seed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AB3C76-FD01-4728-8A77-F4B79FFA6843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A62E1B-8DD3-425A-A703-249EC5BF0434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3F55CF73-28A6-40FE-B0CC-61CC8B8E591E}"/>
   </bookViews>
   <sheets>
     <sheet name="floor_1" sheetId="1" r:id="rId1"/>
+    <sheet name="floor_2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -54,7 +52,97 @@
     <t>place_id</t>
   </si>
   <si>
-    <t>Pizza Company</t>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>Pizza Company 1</t>
+  </si>
+  <si>
+    <t>Pizza Company 2</t>
+  </si>
+  <si>
+    <t>Pizza Company 3</t>
+  </si>
+  <si>
+    <t>Pizza Company 4</t>
+  </si>
+  <si>
+    <t>Pizza Company 5</t>
+  </si>
+  <si>
+    <t>Pizza Company 6</t>
+  </si>
+  <si>
+    <t>Pizza Company 7</t>
+  </si>
+  <si>
+    <t>Pizza Company 8</t>
+  </si>
+  <si>
+    <t>Pizza Company 9</t>
+  </si>
+  <si>
+    <t>Pizza Company 10</t>
+  </si>
+  <si>
+    <t>Pizza Company 11</t>
+  </si>
+  <si>
+    <t>Pizza Company 12</t>
+  </si>
+  <si>
+    <t>Pizza Company 13</t>
+  </si>
+  <si>
+    <t>Pizza Company 14</t>
+  </si>
+  <si>
+    <t>Pizza Company 15</t>
+  </si>
+  <si>
+    <t>Pizza Company 16</t>
+  </si>
+  <si>
+    <t>Pizza Company 17</t>
+  </si>
+  <si>
+    <t>Pizza Company 18</t>
+  </si>
+  <si>
+    <t>Pizza Company 19</t>
+  </si>
+  <si>
+    <t>Pizza Company 20</t>
+  </si>
+  <si>
+    <t>Pizza Company 21</t>
+  </si>
+  <si>
+    <t>Pizza Company 22</t>
+  </si>
+  <si>
+    <t>Pizza Company 23</t>
+  </si>
+  <si>
+    <t>Pizza Company 24</t>
+  </si>
+  <si>
+    <t>Pizza Company 25</t>
+  </si>
+  <si>
+    <t>Pizza Company 26</t>
+  </si>
+  <si>
+    <t>Pizza Company 27</t>
+  </si>
+  <si>
+    <t>Pizza Company 28</t>
+  </si>
+  <si>
+    <t>Pizza Company 29</t>
   </si>
   <si>
     <t>id</t>
@@ -64,10 +152,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -409,20 +503,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB51F8B0-0540-41A5-B6B7-101305F1638E}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -434,21 +529,27 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -457,15 +558,21 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="H2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -474,15 +581,21 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="H3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -491,15 +604,21 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -508,15 +627,21 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -525,15 +650,21 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -542,15 +673,21 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -559,15 +696,21 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="H8">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -576,15 +719,21 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="H9">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -593,15 +742,21 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="H10">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -610,15 +765,21 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="H11">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -627,15 +788,21 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="H12">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -644,15 +811,21 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+      <c r="H13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -661,15 +834,21 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="H14">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -678,15 +857,21 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="H15">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -695,15 +880,21 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="H16">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -712,15 +903,21 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="H17">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>23</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -729,15 +926,21 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+      <c r="H18">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -746,15 +949,21 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+      <c r="H19">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -763,15 +972,21 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+      <c r="H20">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>26</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -780,15 +995,21 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+      <c r="H21">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -797,15 +1018,21 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+      <c r="H22">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -814,15 +1041,21 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+      <c r="H23">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -831,15 +1064,21 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+      <c r="H24">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -848,15 +1087,21 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+      <c r="H25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>31</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -865,15 +1110,21 @@
         <v>1</v>
       </c>
       <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+      <c r="H26">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -882,61 +1133,750 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="H27">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>530</v>
+      </c>
+      <c r="H28">
+        <v>286</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672B1FCA-EEDC-479B-9C1D-BBA383CAFC53}">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>300</v>
+      </c>
+      <c r="H2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>290</v>
+      </c>
+      <c r="H3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>280</v>
+      </c>
+      <c r="H4">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>270</v>
+      </c>
+      <c r="H5">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>260</v>
+      </c>
+      <c r="H6">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>250</v>
+      </c>
+      <c r="H7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>240</v>
+      </c>
+      <c r="H8">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>230</v>
+      </c>
+      <c r="H9">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>220</v>
+      </c>
+      <c r="H10">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>210</v>
+      </c>
+      <c r="H11">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>200</v>
+      </c>
+      <c r="H12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>190</v>
+      </c>
+      <c r="H13">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>180</v>
+      </c>
+      <c r="H14">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>170</v>
+      </c>
+      <c r="H15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>160</v>
+      </c>
+      <c r="H16">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>150</v>
+      </c>
+      <c r="H17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>140</v>
+      </c>
+      <c r="H18">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>130</v>
+      </c>
+      <c r="H19">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>120</v>
+      </c>
+      <c r="H20">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>110</v>
+      </c>
+      <c r="H21">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>90</v>
+      </c>
+      <c r="H23">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>80</v>
+      </c>
+      <c r="H24">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>70</v>
+      </c>
+      <c r="H25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>60</v>
+      </c>
+      <c r="H26">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="H28">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>34</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="H29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="H30">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>